<commit_message>
Added more tests and report listener
</commit_message>
<xml_diff>
--- a/src/test/java/com/framework/testData/TestData.xlsx
+++ b/src/test/java/com/framework/testData/TestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E31686-E57A-45BD-990E-75E6A7F5EA3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CCB3DC-AB4F-449E-96AA-298736D4A701}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="105">
   <si>
     <t>password</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Ward</t>
   </si>
   <si>
-    <t>TC_CreateUsers_002</t>
-  </si>
-  <si>
     <t>Steve</t>
   </si>
   <si>
@@ -285,6 +282,60 @@
   </si>
   <si>
     <t>https://www.GermanShepherd/snap001.jpeg, https://www.GermanShepherd/snap002.jpeg, https://www.GermanShepherd/snap003.jpeg</t>
+  </si>
+  <si>
+    <t>ariz077</t>
+  </si>
+  <si>
+    <t>Brian1000</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>Krish</t>
+  </si>
+  <si>
+    <t>Krish00</t>
+  </si>
+  <si>
+    <t>Das</t>
+  </si>
+  <si>
+    <t>Krish002@hotmail.com</t>
+  </si>
+  <si>
+    <t>something bad happened</t>
+  </si>
+  <si>
+    <t>TC_CreateUser</t>
+  </si>
+  <si>
+    <t>efgh</t>
+  </si>
+  <si>
+    <t>dwayne901</t>
+  </si>
+  <si>
+    <t>Dwayne</t>
+  </si>
+  <si>
+    <t>Johnson</t>
+  </si>
+  <si>
+    <t>dwaynejohnson901@gmail.com</t>
+  </si>
+  <si>
+    <t>statusCode</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>User not found</t>
+  </si>
+  <si>
+    <t>tt</t>
   </si>
 </sst>
 </file>
@@ -781,10 +832,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView topLeftCell="J1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="23.5" x14ac:dyDescent="0.55000000000000004"/>
@@ -798,12 +849,13 @@
     <col min="7" max="7" width="45.7265625" style="15" customWidth="1"/>
     <col min="8" max="8" width="23.1796875" style="15" customWidth="1"/>
     <col min="9" max="9" width="29.6328125" style="7" customWidth="1"/>
-    <col min="10" max="10" width="32.54296875" style="7" customWidth="1"/>
-    <col min="11" max="13" width="24.7265625" style="7" customWidth="1"/>
-    <col min="14" max="16384" width="8.7265625" style="7"/>
+    <col min="10" max="11" width="32.54296875" style="7" customWidth="1"/>
+    <col min="12" max="13" width="24.7265625" style="7" customWidth="1"/>
+    <col min="14" max="14" width="35.453125" style="7" customWidth="1"/>
+    <col min="15" max="16384" width="8.7265625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="8" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:14" s="8" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="9" t="s">
         <v>3</v>
       </c>
@@ -835,21 +887,24 @@
         <v>8</v>
       </c>
       <c r="K1" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="L1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C2" s="13">
         <v>10001</v>
@@ -858,10 +913,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="13" t="s">
         <v>34</v>
-      </c>
-      <c r="F2" s="13" t="s">
-        <v>35</v>
       </c>
       <c r="G2" s="14" t="s">
         <v>15</v>
@@ -878,19 +933,22 @@
       <c r="K2" s="13">
         <v>200</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="13">
+        <v>200</v>
+      </c>
+      <c r="M2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="N2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C3" s="13">
         <v>10002</v>
@@ -902,7 +960,7 @@
         <v>19</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G3" s="14" t="s">
         <v>20</v>
@@ -919,19 +977,22 @@
       <c r="K3" s="13">
         <v>200</v>
       </c>
-      <c r="L3" s="13" t="s">
+      <c r="L3" s="13">
+        <v>200</v>
+      </c>
+      <c r="M3" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M3" s="13" t="s">
+      <c r="N3" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="13">
         <v>10003</v>
@@ -943,7 +1004,7 @@
         <v>22</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G4" s="14" t="s">
         <v>24</v>
@@ -960,37 +1021,40 @@
       <c r="K4" s="13">
         <v>200</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="13">
+        <v>200</v>
+      </c>
+      <c r="M4" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="13" t="s">
+      <c r="N4" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="13" t="s">
-        <v>28</v>
+        <v>95</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="13">
         <v>10004</v>
       </c>
       <c r="D5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="E5" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>32</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>33</v>
       </c>
       <c r="I5" s="13">
         <v>9987456397</v>
@@ -1001,25 +1065,28 @@
       <c r="K5" s="13">
         <v>200</v>
       </c>
-      <c r="L5" s="13" t="s">
+      <c r="L5" s="13">
+        <v>200</v>
+      </c>
+      <c r="M5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M5" s="13" t="s">
+      <c r="N5" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="13">
         <v>10001</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>26</v>
@@ -1042,25 +1109,28 @@
       <c r="K6" s="13">
         <v>200</v>
       </c>
-      <c r="L6" s="13" t="s">
+      <c r="L6" s="13">
+        <v>200</v>
+      </c>
+      <c r="M6" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="13">
+      <c r="N6" s="13">
         <v>10001</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="13" t="s">
         <v>43</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="13">
         <v>10001</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="E7" s="13" t="s">
         <v>26</v>
@@ -1083,37 +1153,40 @@
       <c r="K7" s="13">
         <v>200</v>
       </c>
-      <c r="L7" s="13" t="s">
+      <c r="L7" s="13">
+        <v>200</v>
+      </c>
+      <c r="M7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="13">
+      <c r="N7" s="13">
         <v>10001</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="13">
         <v>10005</v>
       </c>
       <c r="D8" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="F8" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>48</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>49</v>
       </c>
       <c r="I8" s="13">
         <v>9987456388</v>
@@ -1124,37 +1197,40 @@
       <c r="K8" s="13">
         <v>200</v>
       </c>
-      <c r="L8" s="13" t="s">
+      <c r="L8" s="13">
+        <v>200</v>
+      </c>
+      <c r="M8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M8" s="13" t="s">
+      <c r="N8" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="13">
         <v>10006</v>
       </c>
       <c r="D9" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="E9" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" s="14" t="s">
+      <c r="H9" s="14" t="s">
         <v>83</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>84</v>
       </c>
       <c r="I9" s="13">
         <v>9987456666</v>
@@ -1165,37 +1241,40 @@
       <c r="K9" s="13">
         <v>200</v>
       </c>
-      <c r="L9" s="13" t="s">
+      <c r="L9" s="13">
+        <v>200</v>
+      </c>
+      <c r="M9" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M9" s="13" t="s">
+      <c r="N9" s="13" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="13">
         <v>10005</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="E10" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="13" t="s">
+      <c r="G10" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="I10" s="13">
         <v>9987456300</v>
@@ -1206,37 +1285,40 @@
       <c r="K10" s="13">
         <v>200</v>
       </c>
-      <c r="L10" s="13" t="s">
+      <c r="L10" s="13">
+        <v>200</v>
+      </c>
+      <c r="M10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="13">
+      <c r="N10" s="13">
         <v>10005</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="13">
         <v>10005</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="E11" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F11" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="G11" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="H11" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="I11" s="13">
         <v>9987456300</v>
@@ -1247,11 +1329,146 @@
       <c r="K11" s="13">
         <v>200</v>
       </c>
-      <c r="L11" s="13" t="s">
+      <c r="L11" s="13">
+        <v>200</v>
+      </c>
+      <c r="M11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="M11" s="13">
+      <c r="N11" s="13">
         <v>10005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="13">
+        <v>9987456398</v>
+      </c>
+      <c r="J12" s="13">
+        <v>0</v>
+      </c>
+      <c r="K12" s="13">
+        <v>500</v>
+      </c>
+      <c r="L12" s="13">
+        <v>500</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="13">
+        <v>9971766548</v>
+      </c>
+      <c r="J13" s="13">
+        <v>0</v>
+      </c>
+      <c r="K13" s="13">
+        <v>500</v>
+      </c>
+      <c r="L13" s="13">
+        <v>500</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="13">
+        <v>10001</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="H14" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="13">
+        <v>9971766544</v>
+      </c>
+      <c r="J14" s="13">
+        <v>0</v>
+      </c>
+      <c r="K14" s="13">
+        <v>404</v>
+      </c>
+      <c r="L14" s="13">
+        <v>1</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="N14" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1274,18 +1491,22 @@
     <hyperlink ref="H11" r:id="rId15" display="hello4321@" xr:uid="{51D433E2-8B06-4745-809E-D0C33516CD78}"/>
     <hyperlink ref="G9" r:id="rId16" xr:uid="{B710B22C-69C8-4A67-BBC1-708725840D99}"/>
     <hyperlink ref="H9" r:id="rId17" display="hello111@" xr:uid="{727F68BE-7DB9-4054-B58E-90C46E5428A0}"/>
+    <hyperlink ref="G12" r:id="rId18" xr:uid="{C81F0F84-8413-42C8-AB2F-D4F9EAC4111C}"/>
+    <hyperlink ref="H12" r:id="rId19" xr:uid="{61F914AD-9FC6-4C95-8EFC-41597DD1CB06}"/>
+    <hyperlink ref="G13" r:id="rId20" xr:uid="{CAFACC70-2930-4885-894A-ADA72E76BD93}"/>
+    <hyperlink ref="G14" r:id="rId21" xr:uid="{793B94FE-D610-45BF-8B32-0949C0440A7A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3697F6-CEE1-4D70-B6E6-3BCE5BD44B0A}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1298,10 +1519,11 @@
     <col min="6" max="6" width="32.54296875" customWidth="1"/>
     <col min="7" max="7" width="27" style="17" customWidth="1"/>
     <col min="8" max="8" width="23.1796875" customWidth="1"/>
-    <col min="9" max="9" width="70.54296875" customWidth="1"/>
+    <col min="9" max="9" width="20.7265625" customWidth="1"/>
+    <col min="10" max="10" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="6" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="6" customFormat="1" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -1312,30 +1534,33 @@
         <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="H1" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="50" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J1" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="50" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1">
         <v>20001</v>
@@ -1344,27 +1569,30 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="G2" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="18" t="s">
-        <v>65</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J2" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>73</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>74</v>
       </c>
       <c r="C3" s="1">
         <v>20002</v>
@@ -1373,27 +1601,30 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="H3" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="I3" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+        <v>65</v>
+      </c>
+      <c r="J3" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C4" s="1">
         <v>20002</v>
@@ -1402,27 +1633,30 @@
         <v>3</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>87</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4" s="1">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="41.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C5" s="1">
         <v>20002</v>
@@ -1431,19 +1665,22 @@
         <v>3</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>85</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="I5" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="G5" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>80</v>
+      <c r="J5" s="1">
+        <v>200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>